<commit_message>
update graphs and report
</commit_message>
<xml_diff>
--- a/Data/Model 0.0.xlsx
+++ b/Data/Model 0.0.xlsx
@@ -641,6 +641,9 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>95% cooperative</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:noFill/>
@@ -650,7 +653,7 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:size val="3"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
@@ -1292,6 +1295,9 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:v>5% cooperative </c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:noFill/>
@@ -1301,7 +1307,7 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:size val="3"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
@@ -1943,6 +1949,9 @@
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
+          <c:tx>
+            <c:v>67% cooperative </c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:noFill/>
@@ -1952,7 +1961,7 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:size val="3"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent3"/>
@@ -2599,11 +2608,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="453302576"/>
-        <c:axId val="453290424"/>
+        <c:axId val="354009072"/>
+        <c:axId val="354014952"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="453302576"/>
+        <c:axId val="354009072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -2717,12 +2726,12 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="453290424"/>
+        <c:crossAx val="354014952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="453290424"/>
+        <c:axId val="354014952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2842,7 +2851,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="453302576"/>
+        <c:crossAx val="354009072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2854,6 +2863,38 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="nl-NL"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -3451,16 +3492,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>30480</xdr:colOff>
-      <xdr:row>80</xdr:row>
-      <xdr:rowOff>3810</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>121920</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>335280</xdr:colOff>
-      <xdr:row>95</xdr:row>
-      <xdr:rowOff>3810</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>426720</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3747,8 +3788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
-      <selection activeCell="F72" sqref="F72"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>